<commit_message>
Added dynamic dropdown ui functionality
</commit_message>
<xml_diff>
--- a/inputs/Investment_ticker_symbols.xlsx
+++ b/inputs/Investment_ticker_symbols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chris\Documents\Investment_dashboard\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44D4559A-598A-4FF3-811B-CE8D3E9BF298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E026B65E-6665-4DC1-8BCE-66D903910B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{4EF43D60-02D9-47FB-96B7-73E6CDCB0148}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4EF43D60-02D9-47FB-96B7-73E6CDCB0148}"/>
   </bookViews>
   <sheets>
     <sheet name="Stock_list" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="135">
   <si>
     <t>AI.PA</t>
   </si>
@@ -396,6 +396,42 @@
   </si>
   <si>
     <t>Hang Seng Index (Hong Kong Stock Exchange)</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Commodity</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Consumer &amp; Medical Goods</t>
+  </si>
+  <si>
+    <t>Chemical &amp; Functional Materials</t>
+  </si>
+  <si>
+    <t>Cosmetics</t>
+  </si>
+  <si>
+    <t>Food &amp; Fragrances</t>
+  </si>
+  <si>
+    <t>Oil, Gas, &amp; Energy</t>
+  </si>
+  <si>
+    <t>Pharmaceuticals</t>
+  </si>
+  <si>
+    <t>Retailers</t>
   </si>
 </sst>
 </file>
@@ -747,428 +783,599 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5DABCE-A0FC-4D7C-8052-2B9E73BAEABA}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>40</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>42</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>46</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>48</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>49</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>51</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>53</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>55</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>57</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>59</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>61</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>63</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C34" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>65</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>67</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>69</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>71</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C38" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>73</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="C39" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>75</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="C40" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>77</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>79</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="C42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>81</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="C43" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>83</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="C44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>85</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="C45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>87</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="C46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>89</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="C47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>91</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="C48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>93</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="C49" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>95</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="C50" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>97</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="C51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>99</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="C52" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>101</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>102</v>
+      </c>
+      <c r="C53" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1178,91 +1385,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BB014E-0098-4B96-8D90-44F6035FA117}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>121</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1273,12 +1488,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2D88B9-70A2-493F-91E2-E886F624DA05}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Simplified equity data acquisition functions
</commit_message>
<xml_diff>
--- a/inputs/Investment_ticker_symbols.xlsx
+++ b/inputs/Investment_ticker_symbols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chris\Documents\Investment_dashboard\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E026B65E-6665-4DC1-8BCE-66D903910B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B64EE0B-D65E-4DC9-8CA8-0DA7F2ED7821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4EF43D60-02D9-47FB-96B7-73E6CDCB0148}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="163">
   <si>
     <t>AI.PA</t>
   </si>
@@ -432,6 +432,90 @@
   </si>
   <si>
     <t>Retailers</t>
+  </si>
+  <si>
+    <t>Semiconductors</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>NVIDIA</t>
+  </si>
+  <si>
+    <t>iShares Core S&amp;P 500 ETF</t>
+  </si>
+  <si>
+    <t>IVV</t>
+  </si>
+  <si>
+    <t>Exchange-traded fund (ETF)</t>
+  </si>
+  <si>
+    <t>Vanguard US Momentum Factor ETF</t>
+  </si>
+  <si>
+    <t>VFMO</t>
+  </si>
+  <si>
+    <t>iShares MSCI India ETF</t>
+  </si>
+  <si>
+    <t>INDA</t>
+  </si>
+  <si>
+    <t>iShares MSCI China ETF</t>
+  </si>
+  <si>
+    <t>MCHI</t>
+  </si>
+  <si>
+    <t>iShares MSCI World ETF</t>
+  </si>
+  <si>
+    <t>URTH</t>
+  </si>
+  <si>
+    <t>Kenvue</t>
+  </si>
+  <si>
+    <t>KVUE</t>
+  </si>
+  <si>
+    <t>GE Vernova Inc</t>
+  </si>
+  <si>
+    <t>GEV</t>
+  </si>
+  <si>
+    <t>S&amp;P Global</t>
+  </si>
+  <si>
+    <t>SPGI</t>
+  </si>
+  <si>
+    <t>Financial</t>
+  </si>
+  <si>
+    <t>Schrödinger, Inc.</t>
+  </si>
+  <si>
+    <t>SDGR</t>
+  </si>
+  <si>
+    <t>Verizon Communications Inc.</t>
+  </si>
+  <si>
+    <t>Telecommunications</t>
+  </si>
+  <si>
+    <t>VZ</t>
+  </si>
+  <si>
+    <t>The Hershey Company</t>
+  </si>
+  <si>
+    <t>HSY</t>
   </si>
 </sst>
 </file>
@@ -783,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5DABCE-A0FC-4D7C-8052-2B9E73BAEABA}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,21 +1145,21 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>152</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>151</v>
       </c>
       <c r="C25" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>162</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>161</v>
       </c>
       <c r="C26" t="s">
         <v>131</v>
@@ -1083,87 +1167,87 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>139</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>138</v>
       </c>
       <c r="C29" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>146</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>145</v>
       </c>
       <c r="C30" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
       <c r="C31" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>148</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>147</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
         <v>129</v>
@@ -1171,210 +1255,342 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>150</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="C36" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C44" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="C47" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C48" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C50" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C52" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" t="s">
+        <v>156</v>
+      </c>
+      <c r="C54" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64" t="s">
+        <v>158</v>
+      </c>
+      <c r="C64" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>101</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B65" t="s">
         <v>102</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C65" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>